<commit_message>
Updated on 6 Mar 2021
</commit_message>
<xml_diff>
--- a/2wdproj_py37/TSP_Testing.xlsx
+++ b/2wdproj_py37/TSP_Testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yewmun.yip/Documents/creating-grids-in-flask/2wdproj_py37/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yipyewmun/Documents/GitHub/creating-grids-in-flask/2wdproj_py37/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2679100-D3AC-D64C-BC85-9B651DD3A56A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4888A84-CBA3-B940-8D06-AC7EFDE5CFA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{768142CC-7A08-7049-9E40-93542294B2A0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{768142CC-7A08-7049-9E40-93542294B2A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Depot</t>
   </si>
@@ -75,37 +75,73 @@
     <t>Rack L</t>
   </si>
   <si>
-    <t>F, 1</t>
-  </si>
-  <si>
-    <t>H, 2</t>
-  </si>
-  <si>
-    <t>J, 3</t>
-  </si>
-  <si>
-    <t>K, 4</t>
-  </si>
-  <si>
-    <t>I, 5</t>
-  </si>
-  <si>
-    <t>G, 6</t>
-  </si>
-  <si>
-    <t>E, 7</t>
-  </si>
-  <si>
-    <t>A, 8</t>
-  </si>
-  <si>
-    <t>B, 9</t>
-  </si>
-  <si>
-    <t>D, 10</t>
-  </si>
-  <si>
-    <t>C, 11</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>A7, 1</t>
+  </si>
+  <si>
+    <t>A11, 2</t>
+  </si>
+  <si>
+    <t>D9, 3</t>
+  </si>
+  <si>
+    <t>E12, 4</t>
+  </si>
+  <si>
+    <t>H10, 5</t>
+  </si>
+  <si>
+    <t>L12, 6</t>
+  </si>
+  <si>
+    <t>J8, 7</t>
+  </si>
+  <si>
+    <t>F2, 8</t>
+  </si>
+  <si>
+    <t>D3, 9</t>
+  </si>
+  <si>
+    <t>C6, 10</t>
+  </si>
+  <si>
+    <t>B2, 11</t>
   </si>
 </sst>
 </file>
@@ -384,12 +420,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -409,6 +442,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,424 +769,617 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6174336D-6B14-2248-B94D-D05972CE50C7}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="4"/>
-    </row>
-    <row r="2" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="12"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="21" t="s">
+    <row r="1" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="L1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="13"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="13"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="21" t="s">
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="13"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="13"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="13"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="21" t="s">
+      <c r="R1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="21"/>
+      <c r="T1" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="9"/>
+      <c r="D2" s="23">
         <v>13</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="13"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="13"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="13"/>
-    </row>
-    <row r="15" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="14"/>
-    </row>
-    <row r="16" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="7"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="23">
+        <v>13</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="23">
+        <v>13</v>
+      </c>
+      <c r="K2" s="12"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="23">
+        <v>13</v>
+      </c>
+      <c r="N2" s="12"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="23">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="23">
+        <v>13</v>
+      </c>
+      <c r="T2" s="9"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C3" s="10"/>
+      <c r="D3" s="23">
+        <v>12</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="23">
+        <v>12</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="23">
+        <v>12</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="23">
+        <v>12</v>
+      </c>
+      <c r="N3" s="14"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="23">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="23">
+        <v>12</v>
+      </c>
+      <c r="T3" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="23">
+        <v>11</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="23">
+        <v>11</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="23">
+        <v>11</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="23">
+        <v>11</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="23">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="23">
+        <v>11</v>
+      </c>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C5" s="10"/>
+      <c r="D5" s="23">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="23">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="23">
+        <v>10</v>
+      </c>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="23">
+        <v>10</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="15"/>
+      <c r="P5" s="23">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="23">
+        <v>10</v>
+      </c>
+      <c r="T5" s="10"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C6" s="10"/>
+      <c r="D6" s="23">
+        <v>9</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="23">
+        <v>9</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="23">
+        <v>9</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="23">
+        <v>9</v>
+      </c>
+      <c r="N6" s="14"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="23">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="23">
+        <v>9</v>
+      </c>
+      <c r="T6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C7" s="10"/>
+      <c r="D7" s="23">
+        <v>8</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="23">
+        <v>8</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="23">
+        <v>8</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="23">
+        <v>8</v>
+      </c>
+      <c r="N7" s="14"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="23">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" s="15"/>
+      <c r="S7" s="23">
+        <v>8</v>
+      </c>
+      <c r="T7" s="10"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="23">
+        <v>7</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="23">
+        <v>7</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="23">
+        <v>7</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="23">
+        <v>7</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="23">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="23">
+        <v>7</v>
+      </c>
+      <c r="T8" s="10"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C9" s="10"/>
+      <c r="D9" s="23">
+        <v>6</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="23">
+        <v>6</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="23">
+        <v>6</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="23">
+        <v>6</v>
+      </c>
+      <c r="N9" s="14"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="23">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="23">
+        <v>6</v>
+      </c>
+      <c r="T9" s="10"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C10" s="10"/>
+      <c r="D10" s="23">
+        <v>5</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="23">
+        <v>5</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="23">
+        <v>5</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="23">
+        <v>5</v>
+      </c>
+      <c r="N10" s="14"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="23">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="23">
+        <v>5</v>
+      </c>
+      <c r="T10" s="10"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C11" s="10"/>
+      <c r="D11" s="23">
+        <v>4</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="23">
+        <v>4</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="23">
+        <v>4</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="23">
+        <v>4</v>
+      </c>
+      <c r="N11" s="14"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="23">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="23">
+        <v>4</v>
+      </c>
+      <c r="T11" s="10"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C12" s="10"/>
+      <c r="D12" s="23">
+        <v>3</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="23">
+        <v>3</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="23">
+        <v>3</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="23">
+        <v>3</v>
+      </c>
+      <c r="N12" s="14"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="23">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="23">
+        <v>3</v>
+      </c>
+      <c r="T12" s="10"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C13" s="10"/>
+      <c r="D13" s="23">
+        <v>2</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="23">
+        <v>2</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="23">
+        <v>2</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="15"/>
+      <c r="M13" s="23">
+        <v>2</v>
+      </c>
+      <c r="N13" s="14"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="23">
+        <v>2</v>
+      </c>
+      <c r="T13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C14" s="10"/>
+      <c r="D14" s="23">
         <v>1</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="5" t="s">
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="23">
+        <v>1</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="23">
+        <v>1</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="23">
+        <v>1</v>
+      </c>
+      <c r="N14" s="14"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="23">
+        <v>1</v>
+      </c>
+      <c r="T14" s="10"/>
+    </row>
+    <row r="15" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="23">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="23">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="23">
+        <v>0</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="23">
+        <v>0</v>
+      </c>
+      <c r="N15" s="16"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="23">
+        <v>0</v>
+      </c>
+      <c r="T15" s="11"/>
+    </row>
+    <row r="16" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="F17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="L17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="O17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="6" t="s">
+      <c r="P17" s="2"/>
+      <c r="Q17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P17" s="5" t="s">
+      <c r="R17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="7" t="s">
+      <c r="S17" s="2"/>
+      <c r="T17" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="11"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="8"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated on 11 Mar 2021
</commit_message>
<xml_diff>
--- a/2wdproj_py37/TSP_Testing.xlsx
+++ b/2wdproj_py37/TSP_Testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yipyewmun/Documents/GitHub/creating-grids-in-flask/2wdproj_py37/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yewmun.yip/Documents/creating-grids-in-flask/2wdproj_py37/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4888A84-CBA3-B940-8D06-AC7EFDE5CFA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6341250-9466-124A-995B-54F521F14D5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{768142CC-7A08-7049-9E40-93542294B2A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{768142CC-7A08-7049-9E40-93542294B2A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -772,7 +772,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:T18"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1347,7 +1347,7 @@
         <v>9</v>
       </c>
       <c r="P17" s="2"/>
-      <c r="Q17" s="3" t="s">
+      <c r="Q17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="R17" s="2" t="s">

</xml_diff>